<commit_message>
adjusted printing methodology terms
</commit_message>
<xml_diff>
--- a/Printer Materials HU Measurements_v3_publish.xlsx
+++ b/Printer Materials HU Measurements_v3_publish.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwnetid.sharepoint.com/sites/og_rad_3dprinting/Shared Documents/Printing and Modeling Materials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ncross/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="444" documentId="13_ncr:1_{C84C30F6-D2A2-5E44-9642-D55351D7A795}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8DE59C5D-DB82-D84A-ACD9-65CEC200AB7E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{04B9DFBE-C181-2E49-8AAF-EE625F272BBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="980" windowWidth="26880" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6540" yWindow="460" windowWidth="26880" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Data" sheetId="5" r:id="rId1"/>
@@ -983,7 +983,7 @@
     <t>Powder(Plaster+vinyl+sulfate)+Binder(Glycerol+Preservative+Surfactant+water)</t>
   </si>
   <si>
-    <t>PBF</t>
+    <t>BJ</t>
   </si>
   <si>
     <t>http://ytec3d.com/wp-content/uploads/2014/08/zp130.pdf</t>
@@ -1037,7 +1037,7 @@
     <t>FDM=fused deposition modeling</t>
   </si>
   <si>
-    <t>PBF=powder-bond fusion</t>
+    <t>BJ=binder jetting</t>
   </si>
   <si>
     <t>SLA=stereolithography</t>
@@ -1721,8 +1721,8 @@
   <dimension ref="A1:AD1030"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="91" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J112" sqref="J112"/>
+      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L100" sqref="L100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27581,8 +27581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18426040-24E7-654E-832D-FE70C5E0DB22}">
   <dimension ref="A1:W103"/>
   <sheetViews>
-    <sheetView topLeftCell="E22" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView topLeftCell="E91" workbookViewId="0">
+      <selection activeCell="L103" sqref="L103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -36809,7 +36809,7 @@
       </c>
       <c r="L99" s="53" t="str">
         <f>'Material Data'!L99</f>
-        <v>PBF</v>
+        <v>BJ</v>
       </c>
       <c r="M99" s="54">
         <f>'Material Data'!M99</f>
@@ -36903,7 +36903,7 @@
       </c>
       <c r="L100" s="53" t="str">
         <f>'Material Data'!L100</f>
-        <v>PBF</v>
+        <v>BJ</v>
       </c>
       <c r="M100" s="54">
         <f>'Material Data'!M100</f>
@@ -36997,7 +36997,7 @@
       </c>
       <c r="L101" s="53" t="str">
         <f>'Material Data'!L101</f>
-        <v>PBF</v>
+        <v>BJ</v>
       </c>
       <c r="M101" s="54">
         <f>'Material Data'!M101</f>
@@ -37091,7 +37091,7 @@
       </c>
       <c r="L102" s="53" t="str">
         <f>'Material Data'!L102</f>
-        <v>PBF</v>
+        <v>BJ</v>
       </c>
       <c r="M102" s="54">
         <f>'Material Data'!M102</f>
@@ -37185,7 +37185,7 @@
       </c>
       <c r="L103" s="53" t="str">
         <f>'Material Data'!L103</f>
-        <v>PBF</v>
+        <v>BJ</v>
       </c>
       <c r="M103" s="54">
         <f>'Material Data'!M103</f>
@@ -37242,8 +37242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699E3DFB-B1ED-E041-9002-B4D4C339560C}">
   <dimension ref="A1:Y103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AC29" sqref="AC29"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="AE107" sqref="AE107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -41417,7 +41417,7 @@
       </c>
       <c r="D99" s="38" t="str">
         <f>'Material Data'!L99</f>
-        <v>PBF</v>
+        <v>BJ</v>
       </c>
       <c r="E99" s="30"/>
       <c r="F99" s="30"/>
@@ -41456,7 +41456,7 @@
       </c>
       <c r="D100" s="38" t="str">
         <f>'Material Data'!L100</f>
-        <v>PBF</v>
+        <v>BJ</v>
       </c>
       <c r="E100" s="30"/>
       <c r="F100" s="30"/>
@@ -41495,7 +41495,7 @@
       </c>
       <c r="D101" s="38" t="str">
         <f>'Material Data'!L101</f>
-        <v>PBF</v>
+        <v>BJ</v>
       </c>
       <c r="E101" s="30"/>
       <c r="F101" s="30"/>
@@ -41534,7 +41534,7 @@
       </c>
       <c r="D102" s="38" t="str">
         <f>'Material Data'!L102</f>
-        <v>PBF</v>
+        <v>BJ</v>
       </c>
       <c r="E102" s="30"/>
       <c r="F102" s="30"/>
@@ -41573,7 +41573,7 @@
       </c>
       <c r="D103" s="38" t="str">
         <f>'Material Data'!L103</f>
-        <v>PBF</v>
+        <v>BJ</v>
       </c>
       <c r="E103" s="30"/>
       <c r="F103" s="30"/>
@@ -41607,15 +41607,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007CC3E99D3FAC8741BDF66CE2F5ACA9E0" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="73d7109ea0305359bf74563f5fdc8423">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cd64e2e0-ee9b-412f-a9d7-58f1f94fede4" xmlns:ns3="55b49baa-8133-427e-8635-2e23ffc04250" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4df41ee0fa331ba9a427a2cabea6496a" ns2:_="" ns3:_="">
     <xsd:import namespace="cd64e2e0-ee9b-412f-a9d7-58f1f94fede4"/>
@@ -41832,6 +41823,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -41839,14 +41839,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E819515-85E7-4355-AF2A-91D1A9243C50}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{764946F0-8E7F-4474-932A-F30B97950F71}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -41865,16 +41857,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E819515-85E7-4355-AF2A-91D1A9243C50}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8F6F1F5-C61D-42C4-89EB-42C847E676FA}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="55b49baa-8133-427e-8635-2e23ffc04250"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="cd64e2e0-ee9b-412f-a9d7-58f1f94fede4"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="cd64e2e0-ee9b-412f-a9d7-58f1f94fede4"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>

</xml_diff>